<commit_message>
Gephi input and output
Data files and projects for Gephi (complex networks)
</commit_message>
<xml_diff>
--- a/Differentiation Tree Dataset/differentiation-tree-all-variables.xlsx
+++ b/Differentiation Tree Dataset/differentiation-tree-all-variables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5761" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5759" uniqueCount="654">
   <si>
     <t>X</t>
   </si>
@@ -1983,6 +1983,9 @@
   </si>
   <si>
     <t>Larger Cells Above Threshold (+/- 0.5)</t>
+  </si>
+  <si>
+    <t>Mspap</t>
   </si>
 </sst>
 </file>
@@ -2375,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK20" sqref="AK20"/>
+    <sheetView tabSelected="1" topLeftCell="E187" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S224" sqref="S224:U224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2798,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="P5">
-        <v>23.027641819875139</v>
+        <v>23.0276418198751</v>
       </c>
       <c r="Q5">
         <v>0.46842807012183835</v>
@@ -7666,7 +7669,18 @@
       <c r="E61" s="3">
         <v>14.650432595</v>
       </c>
-      <c r="F61" s="5"/>
+      <c r="F61" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="G61" s="2">
+        <v>371.51993107500004</v>
+      </c>
+      <c r="H61" s="2">
+        <v>239.53510750000001</v>
+      </c>
+      <c r="I61" s="2">
+        <v>14.5626457275</v>
+      </c>
       <c r="J61" s="6" t="s">
         <v>517</v>
       </c>
@@ -7682,14 +7696,14 @@
       <c r="O61">
         <v>60</v>
       </c>
-      <c r="P61" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>2</v>
-      </c>
-      <c r="R61" t="s">
-        <v>2</v>
+      <c r="P61">
+        <v>5.9825950620613186</v>
+      </c>
+      <c r="Q61">
+        <v>1.0159212033913629</v>
+      </c>
+      <c r="R61">
+        <v>0.10647664825611244</v>
       </c>
       <c r="S61">
         <v>52.356193602863762</v>
@@ -7706,21 +7720,23 @@
       <c r="X61" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="Y61" s="5"/>
+      <c r="Y61" s="5" t="s">
+        <v>653</v>
+      </c>
       <c r="Z61" s="6" t="s">
         <v>517</v>
       </c>
       <c r="AA61" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AB61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC61">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="AD61" s="12" t="s">
-        <v>517</v>
+        <v>653</v>
       </c>
       <c r="AE61" s="13"/>
     </row>
@@ -19302,9 +19318,6 @@
       <c r="R205" t="s">
         <v>2</v>
       </c>
-      <c r="S205" t="s">
-        <v>2</v>
-      </c>
       <c r="T205" t="s">
         <v>2</v>
       </c>

</xml_diff>